<commit_message>
add roles in project correct
</commit_message>
<xml_diff>
--- a/tacy_app/media/files/user/1/reestr.xlsx
+++ b/tacy_app/media/files/user/1/reestr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>№</t>
   </si>
@@ -25,34 +25,31 @@
     <t>Статус</t>
   </si>
   <si>
-    <t>d</t>
+    <t>й</t>
+  </si>
+  <si>
+    <t>ц</t>
+  </si>
+  <si>
+    <t>ы2</t>
+  </si>
+  <si>
+    <t>ыы</t>
   </si>
   <si>
     <t>s</t>
   </si>
   <si>
-    <t>d11</t>
-  </si>
-  <si>
-    <t>d12</t>
-  </si>
-  <si>
-    <t>ss</t>
-  </si>
-  <si>
-    <t>ц</t>
-  </si>
-  <si>
     <t>Согласовано</t>
   </si>
   <si>
-    <t>d1</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>fF f.f</t>
+    <t>й1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Хватов ы.ы; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">null null.null; Y s.s; </t>
   </si>
 </sst>
 </file>
@@ -103,17 +100,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H2" totalsRowShown="0">
-  <autoFilter ref="A1:H2"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G2" totalsRowShown="0">
+  <autoFilter ref="A1:G2"/>
+  <tableColumns count="7">
     <tableColumn id="1" name="№"/>
     <tableColumn id="2" name="Название инициативы"/>
     <tableColumn id="3" name="Статус"/>
-    <tableColumn id="4" name="d"/>
-    <tableColumn id="5" name="s"/>
-    <tableColumn id="6" name="d11"/>
-    <tableColumn id="7" name="d12"/>
-    <tableColumn id="8" name="ss"/>
+    <tableColumn id="4" name="й"/>
+    <tableColumn id="5" name="ц"/>
+    <tableColumn id="6" name="ы2"/>
+    <tableColumn id="7" name="ыы"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -404,7 +400,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,10 +408,10 @@
   <cols>
     <col min="1" max="1" width="5.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="45.7109375" style="1" customWidth="1"/>
-    <col min="3" max="9" width="25.7109375" style="1" customWidth="1"/>
+    <col min="3" max="8" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,34 +433,28 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1">
-        <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v 2.0 go test
</commit_message>
<xml_diff>
--- a/tacy_app/media/files/user/1/reestr.xlsx
+++ b/tacy_app/media/files/user/1/reestr.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="52">
   <si>
     <t>№</t>
   </si>
@@ -70,31 +70,106 @@
     <t>Умное производство,Необходимо уточнить,</t>
   </si>
   <si>
+    <t xml:space="preserve">Соболев А.А; null null.null; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Каковкин П.П; </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шиляков А.А; </t>
+  </si>
+  <si>
+    <t>Ремонт и доведение до проектного состояния ДФМ и вагоноопрокидывателя №2</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Подразделение 1,</t>
+  </si>
+  <si>
+    <t>ДРК,</t>
+  </si>
+  <si>
     <t xml:space="preserve">Соболев А.А; </t>
   </si>
   <si>
-    <t xml:space="preserve">Каковкин П.П; </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Шиляков А.А; </t>
-  </si>
-  <si>
-    <t>Ремонт и доведение до проектного состояния ДФМ и вагоноопрокидывателя №2</t>
+    <t>Ревизия существующей системы пневмообрушения закрытых складов углей (дозировочных отделений №1-№2). Ремонт по результатам ревизии.</t>
   </si>
   <si>
     <t>L0</t>
   </si>
   <si>
-    <t>Подразделение 1,</t>
-  </si>
-  <si>
-    <t>ДРК,</t>
-  </si>
-  <si>
-    <t>Ревизия существующей системы пневмообрушения закрытых складов углей (дозировочных отделений №1-№2). Ремонт по результатам ревизии.</t>
-  </si>
-  <si>
     <t>ДРК,УПП,ЦЕХ,</t>
+  </si>
+  <si>
+    <t>Перевод управления перекидными клапанами (шиберами) с местных пультов управления на центральные пульты управления.</t>
+  </si>
+  <si>
+    <t>Этап 2,</t>
+  </si>
+  <si>
+    <t>УПП,</t>
+  </si>
+  <si>
+    <t>Дооснащение конвейеров оборудованием (резервные приводы, системы плавного пуска, центрирующие опоры роликов, скребки грубой очистки, датчики схода и целостности ленты)</t>
+  </si>
+  <si>
+    <t>УПП,ЦЕХ,ДАТП,Необходимо уточнить,</t>
+  </si>
+  <si>
+    <t>Установка побудителей схода (вибраторов) на металлоконструкции перегрузочных станций.</t>
+  </si>
+  <si>
+    <t>ДРК,ЦЕХ,Необходимо уточнить,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Соболев А.А; Шиляков А.А; Каковкин П.П; </t>
+  </si>
+  <si>
+    <t>Установка пассажирских подъемников в ДО №1, №2, на кранах открытого склада углей.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Каковкин П.П; Шиляков А.А; </t>
+  </si>
+  <si>
+    <t>Пылеподавление на дозаторах ДО №№1, 2</t>
+  </si>
+  <si>
+    <t>Умное производство,ДРК,ЦЕХ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Каковкин П.П; Шиляков А.А; Соболев А.А; </t>
+  </si>
+  <si>
+    <t>Установка датчиков температуры в бункерах</t>
+  </si>
+  <si>
+    <t>ДРК,ЦЕХ,ДАТП,</t>
+  </si>
+  <si>
+    <t>Техническое перевооружение существующих вентиляционных установок и установка новых аспирационных систем</t>
+  </si>
+  <si>
+    <t>Умное производство,УПП,ЦЕХ,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Соболев А.А; Шиляков А.А; </t>
+  </si>
+  <si>
+    <t>Укрытие открытого склада углей  сетчатым забором с 3 сторон</t>
+  </si>
+  <si>
+    <t>Установка системы определения номеров вагонов и передачей информации на пульт оператора вагоноопрокидывателя</t>
+  </si>
+  <si>
+    <t>Умное производство,ДРК,ЦЕХ,ДАТП,</t>
+  </si>
+  <si>
+    <t>Система видеонаблюдения для контроля перемещения персонала и технологического оборудования по открытому складу углей</t>
+  </si>
+  <si>
+    <t>ДРК,УПП,ДАТП,</t>
   </si>
 </sst>
 </file>
@@ -145,8 +220,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M4" totalsRowShown="0">
-  <autoFilter ref="A1:M4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:M14" totalsRowShown="0">
+  <autoFilter ref="A1:M14"/>
   <tableColumns count="13">
     <tableColumn id="1" name="№"/>
     <tableColumn id="2" name="Название инициативы"/>
@@ -451,7 +526,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -523,16 +598,16 @@
         <v>17</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J2" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>18</v>
@@ -579,7 +654,7 @@
         <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>20</v>
@@ -590,10 +665,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>23</v>
@@ -602,7 +677,7 @@
         <v>16</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
@@ -620,7 +695,393 @@
         <v>19</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>36</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="1">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="1">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="1">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="1">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="1">
+        <v>41</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="1">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="1">
+        <v>43</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="1">
+        <v>44</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+      <c r="J13" s="1">
+        <v>0</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="1">
+        <v>45</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+      <c r="J14" s="1">
+        <v>0</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>